<commit_message>
Added alert status checking
</commit_message>
<xml_diff>
--- a/river monitor serial codes.xlsx
+++ b/river monitor serial codes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cyphred\Documents\Arduino\arduino-river-monitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5DBEAA53-7181-4EDA-93A6-0DF8CF947E46}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302E7050-92B1-419D-916A-B4FD631AC846}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34890" yWindow="3240" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="30285" yWindow="2910" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,12 @@
     <sheet name="setting codes" sheetId="4" r:id="rId4"/>
     <sheet name="Activity Log Code" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="47">
   <si>
     <t>Code</t>
   </si>
@@ -162,12 +162,15 @@
   </si>
   <si>
     <t>Sending live reading</t>
+  </si>
+  <si>
+    <t>Check alert mode status</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="15">
     <font>
       <sz val="11"/>
@@ -366,24 +369,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="18">
-    <cellStyle name="Accent" xfId="7"/>
-    <cellStyle name="Accent 1" xfId="8"/>
-    <cellStyle name="Accent 2" xfId="9"/>
-    <cellStyle name="Accent 3" xfId="10"/>
+    <cellStyle name="Accent" xfId="7" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Accent 1" xfId="8" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Accent 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Accent 3" xfId="10" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Bad" xfId="4" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Error" xfId="11"/>
-    <cellStyle name="Footnote" xfId="12"/>
+    <cellStyle name="Error" xfId="11" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Footnote" xfId="12" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Good" xfId="3" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading" xfId="13"/>
+    <cellStyle name="Heading" xfId="13" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="2" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="14"/>
+    <cellStyle name="Hyperlink" xfId="14" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
     <cellStyle name="Neutral" xfId="5" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Note" xfId="6" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Status" xfId="15"/>
-    <cellStyle name="Text" xfId="16"/>
-    <cellStyle name="Warning" xfId="17"/>
+    <cellStyle name="Status" xfId="15" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Text" xfId="16" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Warning" xfId="17" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -694,21 +697,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFD36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AMJ36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="10.625" style="2" customWidth="1"/>
     <col min="2" max="2" width="43.125" style="3" customWidth="1"/>
     <col min="3" max="1024" width="10.625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1022" ht="14.25">
+    <row r="1" spans="1:1022">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -719,7 +722,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:1022" ht="14.25">
+    <row r="2" spans="1:1022">
       <c r="A2" s="2">
         <v>128</v>
       </c>
@@ -1583,7 +1586,7 @@
       <c r="AME2" s="3"/>
       <c r="AMH2" s="3"/>
     </row>
-    <row r="3" spans="1:1022" ht="14.25">
+    <row r="3" spans="1:1022">
       <c r="A3" s="2">
         <v>129</v>
       </c>
@@ -1594,7 +1597,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:1022" ht="14.25">
+    <row r="4" spans="1:1022">
       <c r="A4" s="4">
         <v>130</v>
       </c>
@@ -1605,7 +1608,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:1022" ht="14.25">
+    <row r="5" spans="1:1022">
       <c r="A5" s="2">
         <v>131</v>
       </c>
@@ -1616,7 +1619,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:1022" ht="14.25">
+    <row r="6" spans="1:1022">
       <c r="A6" s="2">
         <v>132</v>
       </c>
@@ -1627,7 +1630,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:1022" ht="14.25">
+    <row r="7" spans="1:1022">
       <c r="A7" s="2">
         <v>133</v>
       </c>
@@ -1638,7 +1641,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1022" ht="14.25">
+    <row r="8" spans="1:1022">
       <c r="A8" s="2">
         <v>134</v>
       </c>
@@ -1649,7 +1652,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:1022" ht="14.25">
+    <row r="9" spans="1:1022">
       <c r="A9" s="2">
         <v>135</v>
       </c>
@@ -1660,7 +1663,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:1022" ht="14.25">
+    <row r="10" spans="1:1022">
       <c r="A10" s="2">
         <v>136</v>
       </c>
@@ -1671,7 +1674,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:1022" ht="14.25">
+    <row r="11" spans="1:1022">
       <c r="A11" s="2">
         <v>137</v>
       </c>
@@ -1682,7 +1685,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:1022" ht="14.25">
+    <row r="12" spans="1:1022">
       <c r="A12" s="2">
         <v>138</v>
       </c>
@@ -1693,7 +1696,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:1022" ht="14.25">
+    <row r="13" spans="1:1022">
       <c r="A13" s="2">
         <v>139</v>
       </c>
@@ -1704,7 +1707,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:1022" ht="14.25">
+    <row r="14" spans="1:1022">
       <c r="A14" s="2">
         <v>140</v>
       </c>
@@ -1715,7 +1718,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:1022" ht="14.25">
+    <row r="15" spans="1:1022">
       <c r="A15" s="2">
         <v>141</v>
       </c>
@@ -1726,7 +1729,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:1022" ht="14.25">
+    <row r="16" spans="1:1022">
       <c r="A16" s="2">
         <v>142</v>
       </c>
@@ -1737,7 +1740,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="14.25">
+    <row r="17" spans="1:3">
       <c r="A17" s="2">
         <v>143</v>
       </c>
@@ -1748,7 +1751,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.25">
+    <row r="18" spans="1:3">
       <c r="A18" s="2">
         <v>144</v>
       </c>
@@ -1759,7 +1762,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="14.25">
+    <row r="19" spans="1:3">
       <c r="A19" s="2">
         <v>145</v>
       </c>
@@ -1770,7 +1773,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="14.25">
+    <row r="20" spans="1:3">
       <c r="A20" s="2">
         <v>146</v>
       </c>
@@ -1781,7 +1784,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="14.25">
+    <row r="21" spans="1:3">
       <c r="A21" s="2">
         <v>147</v>
       </c>
@@ -1792,7 +1795,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="14.25">
+    <row r="22" spans="1:3">
       <c r="A22" s="2">
         <v>148</v>
       </c>
@@ -1803,7 +1806,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="14.25">
+    <row r="23" spans="1:3">
       <c r="A23" s="2">
         <v>149</v>
       </c>
@@ -1814,7 +1817,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="14.25">
+    <row r="24" spans="1:3">
       <c r="A24" s="2">
         <v>150</v>
       </c>
@@ -1825,7 +1828,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="14.25">
+    <row r="25" spans="1:3">
       <c r="A25" s="2">
         <v>151</v>
       </c>
@@ -1836,7 +1839,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="14.25">
+    <row r="26" spans="1:3">
       <c r="A26" s="2">
         <v>152</v>
       </c>
@@ -1847,52 +1850,58 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="14.25">
+    <row r="27" spans="1:3">
       <c r="A27" s="2">
         <v>153</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="14.25">
+      <c r="B27" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" s="2">
         <v>154</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="14.25">
+    <row r="29" spans="1:3">
       <c r="A29" s="2">
         <v>155</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="14.25">
+    <row r="30" spans="1:3">
       <c r="A30" s="2">
         <v>156</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="14.25">
+    <row r="31" spans="1:3">
       <c r="A31" s="2">
         <v>157</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="14.25">
+    <row r="32" spans="1:3">
       <c r="A32" s="2">
         <v>158</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="14.25">
+    <row r="33" spans="1:1">
       <c r="A33" s="2">
         <v>159</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="14.25">
+    <row r="34" spans="1:1">
       <c r="A34" s="2">
         <v>160</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="14.25">
+    <row r="35" spans="1:1">
       <c r="A35" s="2">
         <v>161</v>
       </c>
     </row>
-    <row r="36" spans="1:1" ht="14.25">
+    <row r="36" spans="1:1">
       <c r="A36" s="2">
         <v>162</v>
       </c>
@@ -1907,19 +1916,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFD16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AMJ16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="10.625" style="2" customWidth="1"/>
     <col min="2" max="2" width="43.125" style="3" customWidth="1"/>
     <col min="3" max="1024" width="10.625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1022" ht="14.25">
+    <row r="1" spans="1:1022">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1928,7 +1937,7 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:1022" ht="14.25">
+    <row r="2" spans="1:1022">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -2276,7 +2285,7 @@
       <c r="AME2" s="3"/>
       <c r="AMH2" s="3"/>
     </row>
-    <row r="3" spans="1:1022" ht="14.25">
+    <row r="3" spans="1:1022">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -2284,7 +2293,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:1022" ht="14.25">
+    <row r="4" spans="1:1022">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -2292,7 +2301,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:1022" ht="14.25">
+    <row r="5" spans="1:1022">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -2300,7 +2309,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:1022" ht="14.25">
+    <row r="6" spans="1:1022">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -2308,7 +2317,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:1022" ht="14.25">
+    <row r="7" spans="1:1022">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -2316,31 +2325,31 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:1022" ht="14.25">
+    <row r="8" spans="1:1022">
       <c r="B8" s="5"/>
     </row>
-    <row r="9" spans="1:1022" ht="14.25">
+    <row r="9" spans="1:1022">
       <c r="B9" s="5"/>
     </row>
-    <row r="10" spans="1:1022" ht="14.25">
+    <row r="10" spans="1:1022">
       <c r="B10" s="5"/>
     </row>
-    <row r="11" spans="1:1022" ht="14.25">
+    <row r="11" spans="1:1022">
       <c r="B11" s="6"/>
     </row>
-    <row r="12" spans="1:1022" ht="14.25">
+    <row r="12" spans="1:1022">
       <c r="B12" s="6"/>
     </row>
-    <row r="13" spans="1:1022" ht="14.25">
+    <row r="13" spans="1:1022">
       <c r="B13" s="6"/>
     </row>
-    <row r="14" spans="1:1022" ht="14.25">
+    <row r="14" spans="1:1022">
       <c r="B14" s="6"/>
     </row>
-    <row r="15" spans="1:1022" ht="14.25">
+    <row r="15" spans="1:1022">
       <c r="B15" s="6"/>
     </row>
-    <row r="16" spans="1:1022" ht="14.25">
+    <row r="16" spans="1:1022">
       <c r="B16" s="6"/>
     </row>
   </sheetData>
@@ -2353,19 +2362,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFD16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:AMJ16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="10.625" style="2" customWidth="1"/>
     <col min="2" max="2" width="43.125" style="3" customWidth="1"/>
     <col min="3" max="1024" width="10.625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1022" ht="14.25">
+    <row r="1" spans="1:1022">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2374,7 +2383,7 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:1022" ht="14.25">
+    <row r="2" spans="1:1022">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -2722,7 +2731,7 @@
       <c r="AME2" s="3"/>
       <c r="AMH2" s="3"/>
     </row>
-    <row r="3" spans="1:1022" ht="14.25">
+    <row r="3" spans="1:1022">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -2730,43 +2739,43 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:1022" ht="14.25">
+    <row r="4" spans="1:1022">
       <c r="B4" s="5"/>
     </row>
-    <row r="5" spans="1:1022" ht="14.25">
+    <row r="5" spans="1:1022">
       <c r="B5" s="5"/>
     </row>
-    <row r="6" spans="1:1022" ht="14.25">
+    <row r="6" spans="1:1022">
       <c r="B6" s="5"/>
     </row>
-    <row r="7" spans="1:1022" ht="14.25">
+    <row r="7" spans="1:1022">
       <c r="B7" s="5"/>
     </row>
-    <row r="8" spans="1:1022" ht="14.25">
+    <row r="8" spans="1:1022">
       <c r="B8" s="5"/>
     </row>
-    <row r="9" spans="1:1022" ht="14.25">
+    <row r="9" spans="1:1022">
       <c r="B9" s="5"/>
     </row>
-    <row r="10" spans="1:1022" ht="14.25">
+    <row r="10" spans="1:1022">
       <c r="B10" s="5"/>
     </row>
-    <row r="11" spans="1:1022" ht="14.25">
+    <row r="11" spans="1:1022">
       <c r="B11" s="6"/>
     </row>
-    <row r="12" spans="1:1022" ht="14.25">
+    <row r="12" spans="1:1022">
       <c r="B12" s="6"/>
     </row>
-    <row r="13" spans="1:1022" ht="14.25">
+    <row r="13" spans="1:1022">
       <c r="B13" s="6"/>
     </row>
-    <row r="14" spans="1:1022" ht="14.25">
+    <row r="14" spans="1:1022">
       <c r="B14" s="6"/>
     </row>
-    <row r="15" spans="1:1022" ht="14.25">
+    <row r="15" spans="1:1022">
       <c r="B15" s="6"/>
     </row>
-    <row r="16" spans="1:1022" ht="14.25">
+    <row r="16" spans="1:1022">
       <c r="B16" s="6"/>
     </row>
   </sheetData>
@@ -2779,19 +2788,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFD16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:AMJ16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="10.625" style="2" customWidth="1"/>
     <col min="2" max="2" width="43.125" style="3" customWidth="1"/>
     <col min="3" max="1024" width="10.625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1022" ht="14.25">
+    <row r="1" spans="1:1022">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2800,7 +2809,7 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:1022" ht="14.25">
+    <row r="2" spans="1:1022">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -3148,7 +3157,7 @@
       <c r="AME2" s="3"/>
       <c r="AMH2" s="3"/>
     </row>
-    <row r="3" spans="1:1022" ht="14.25">
+    <row r="3" spans="1:1022">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -3156,7 +3165,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:1022" ht="14.25">
+    <row r="4" spans="1:1022">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -3164,7 +3173,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:1022" ht="14.25">
+    <row r="5" spans="1:1022">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -3172,7 +3181,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:1022" ht="14.25">
+    <row r="6" spans="1:1022">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -3180,7 +3189,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:1022" ht="14.25">
+    <row r="7" spans="1:1022">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -3188,31 +3197,31 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:1022" ht="14.25">
+    <row r="8" spans="1:1022">
       <c r="B8" s="5"/>
     </row>
-    <row r="9" spans="1:1022" ht="14.25">
+    <row r="9" spans="1:1022">
       <c r="B9" s="5"/>
     </row>
-    <row r="10" spans="1:1022" ht="14.25">
+    <row r="10" spans="1:1022">
       <c r="B10" s="5"/>
     </row>
-    <row r="11" spans="1:1022" ht="14.25">
+    <row r="11" spans="1:1022">
       <c r="B11" s="6"/>
     </row>
-    <row r="12" spans="1:1022" ht="14.25">
+    <row r="12" spans="1:1022">
       <c r="B12" s="6"/>
     </row>
-    <row r="13" spans="1:1022" ht="14.25">
+    <row r="13" spans="1:1022">
       <c r="B13" s="6"/>
     </row>
-    <row r="14" spans="1:1022" ht="14.25">
+    <row r="14" spans="1:1022">
       <c r="B14" s="6"/>
     </row>
-    <row r="15" spans="1:1022" ht="14.25">
+    <row r="15" spans="1:1022">
       <c r="B15" s="6"/>
     </row>
-    <row r="16" spans="1:1022" ht="14.25">
+    <row r="16" spans="1:1022">
       <c r="B16" s="6"/>
     </row>
   </sheetData>
@@ -3225,19 +3234,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFD16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:AMJ16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="10.625" style="2" customWidth="1"/>
     <col min="2" max="2" width="43.125" style="3" customWidth="1"/>
     <col min="3" max="1024" width="10.625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1022" ht="14.25">
+    <row r="1" spans="1:1022">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3246,7 +3255,7 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:1022" ht="14.25">
+    <row r="2" spans="1:1022">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -3594,7 +3603,7 @@
       <c r="AME2" s="3"/>
       <c r="AMH2" s="3"/>
     </row>
-    <row r="3" spans="1:1022" ht="14.25">
+    <row r="3" spans="1:1022">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -3602,7 +3611,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:1022" ht="14.25">
+    <row r="4" spans="1:1022">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3610,40 +3619,40 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:1022" ht="14.25">
+    <row r="5" spans="1:1022">
       <c r="B5" s="5"/>
     </row>
-    <row r="6" spans="1:1022" ht="14.25">
+    <row r="6" spans="1:1022">
       <c r="B6" s="5"/>
     </row>
-    <row r="7" spans="1:1022" ht="14.25">
+    <row r="7" spans="1:1022">
       <c r="B7" s="5"/>
     </row>
-    <row r="8" spans="1:1022" ht="14.25">
+    <row r="8" spans="1:1022">
       <c r="B8" s="5"/>
     </row>
-    <row r="9" spans="1:1022" ht="14.25">
+    <row r="9" spans="1:1022">
       <c r="B9" s="5"/>
     </row>
-    <row r="10" spans="1:1022" ht="14.25">
+    <row r="10" spans="1:1022">
       <c r="B10" s="5"/>
     </row>
-    <row r="11" spans="1:1022" ht="14.25">
+    <row r="11" spans="1:1022">
       <c r="B11" s="6"/>
     </row>
-    <row r="12" spans="1:1022" ht="14.25">
+    <row r="12" spans="1:1022">
       <c r="B12" s="6"/>
     </row>
-    <row r="13" spans="1:1022" ht="14.25">
+    <row r="13" spans="1:1022">
       <c r="B13" s="6"/>
     </row>
-    <row r="14" spans="1:1022" ht="14.25">
+    <row r="14" spans="1:1022">
       <c r="B14" s="6"/>
     </row>
-    <row r="15" spans="1:1022" ht="14.25">
+    <row r="15" spans="1:1022">
       <c r="B15" s="6"/>
     </row>
-    <row r="16" spans="1:1022" ht="14.25">
+    <row r="16" spans="1:1022">
       <c r="B16" s="6"/>
     </row>
   </sheetData>

</xml_diff>